<commit_message>
Fixing eeprom settings and naming conventions in controller
</commit_message>
<xml_diff>
--- a/Documentation/ErrorCodes.xlsx
+++ b/Documentation/ErrorCodes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koyug\Documents\GitHub\ArduinoIrrigationController\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFCE629-4863-4894-940F-72A411F8C871}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884ED8C9-F3C7-489B-B89A-17CC266B9109}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{F9656F9B-CE01-44F7-AD78-54935E843959}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Error Code</t>
   </si>
@@ -51,33 +51,18 @@
     <t>The controller received a packet from an address that is not a slave unit or no address was given</t>
   </si>
   <si>
-    <t>errInvalidAddress</t>
-  </si>
-  <si>
-    <t>errPacketLength</t>
-  </si>
-  <si>
     <t>The packet is the wrong length for what is expected</t>
   </si>
   <si>
     <t>Controller and Slaves</t>
   </si>
   <si>
-    <t>errUnkownCommand</t>
-  </si>
-  <si>
-    <t>errUnkownParameters</t>
-  </si>
-  <si>
     <t>The received packet contains a command that the receiving device does not know about or support</t>
   </si>
   <si>
     <t>Some or all of the parameters given in the packet are out of range.</t>
   </si>
   <si>
-    <t>errOutsideRange</t>
-  </si>
-  <si>
     <t>A number is outside the allowed range</t>
   </si>
   <si>
@@ -120,13 +105,37 @@
     <t>The number that was outside the range</t>
   </si>
   <si>
-    <t>errUnexpectedPacket</t>
-  </si>
-  <si>
     <t>We was not expecting stuffs from someonez elses.</t>
   </si>
   <si>
     <t>The address that the packet came from</t>
+  </si>
+  <si>
+    <t>ERR_INVALID_ADDRESS</t>
+  </si>
+  <si>
+    <t>ERR_PACKET_LENGTH</t>
+  </si>
+  <si>
+    <t>ERR_UNKOWN_COMMAND</t>
+  </si>
+  <si>
+    <t>ERR_UNKOWN_PARAMETERS</t>
+  </si>
+  <si>
+    <t>ERR_OUTSIDE_RANGE</t>
+  </si>
+  <si>
+    <t>ERR_UNEXPECTED_PACKET</t>
+  </si>
+  <si>
+    <t>ERR_UNDERVOLTAGE</t>
+  </si>
+  <si>
+    <t>The 5v supply voltage has dropped unexpectedly.</t>
+  </si>
+  <si>
+    <t>The supply voltage (in mV)</t>
   </si>
 </sst>
 </file>
@@ -496,7 +505,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,7 +539,7 @@
         <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -547,16 +556,16 @@
         <v>51</v>
       </c>
       <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -564,13 +573,13 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -578,13 +587,13 @@
         <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -592,13 +601,13 @@
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -606,18 +615,32 @@
         <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -625,13 +648,13 @@
         <v>101</v>
       </c>
       <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
         <v>18</v>
-      </c>
-      <c r="C14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -639,10 +662,10 @@
         <v>102</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -650,13 +673,13 @@
         <v>104</v>
       </c>
       <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
         <v>20</v>
       </c>
-      <c r="C16" t="s">
-        <v>25</v>
-      </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>